<commit_message>
adding another notebooks for image classification
</commit_message>
<xml_diff>
--- a/data/nutrition data/Dataset makanan per 100 gram.xlsx
+++ b/data/nutrition data/Dataset makanan per 100 gram.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CODING\Project Capstone Bisa AI\data\nutrition data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39CEFD74-F32A-486D-99EC-C106F001FAB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD1E0470-825D-4396-A490-5178DD69E14A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1515" yWindow="4995" windowWidth="21660" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
   <si>
     <t>Makanan</t>
   </si>
@@ -107,6 +107,15 @@
   </si>
   <si>
     <t>Ayam_betutu</t>
+  </si>
+  <si>
+    <t>1.8</t>
+  </si>
+  <si>
+    <t>4.8</t>
+  </si>
+  <si>
+    <t>2.4</t>
   </si>
 </sst>
 </file>
@@ -396,7 +405,7 @@
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -480,11 +489,11 @@
       <c r="I2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="3">
-        <v>45505</v>
-      </c>
-      <c r="K2" s="3">
-        <v>45508</v>
+      <c r="J2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="L2" s="2">
         <v>670</v>
@@ -629,8 +638,8 @@
       <c r="H6" s="2">
         <v>287</v>
       </c>
-      <c r="I6" s="3">
-        <v>45384</v>
+      <c r="I6" s="3" t="s">
+        <v>31</v>
       </c>
       <c r="J6" s="2">
         <v>24</v>

</xml_diff>